<commit_message>
Actualización documentación 11 Sep
Actualización documentación 11 Sep
</commit_message>
<xml_diff>
--- a/Bases de datos/DIAGRAMA_RELACIONAL.xlsx
+++ b/Bases de datos/DIAGRAMA_RELACIONAL.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jposa\OneDrive - BQS\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\GitHub\Proyecto_Grupo_3-\Bases de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C08A1374-F5F0-4680-81D7-B25367C739CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{796EA25A-3CFA-43AD-AF04-27E03E5FA6FE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -70,31 +69,31 @@
     <t>CEDULA_usuario (FK)</t>
   </si>
   <si>
-    <t>DESCRIPCION_venta</t>
-  </si>
-  <si>
-    <t>IMAGEN_venta</t>
-  </si>
-  <si>
-    <t>PRECIO_venta</t>
-  </si>
-  <si>
-    <t>FECHA_estado</t>
-  </si>
-  <si>
-    <t>ESTADO (accion comprar,regalar,vender)</t>
-  </si>
-  <si>
-    <t>TIPOPRODUCTO_venta (PK)</t>
-  </si>
-  <si>
     <t>TIPOPRODUCTO_venta (FK)</t>
+  </si>
+  <si>
+    <t>canasta (accion comprar,regalar,vender)</t>
+  </si>
+  <si>
+    <t>FECHA_canasta</t>
+  </si>
+  <si>
+    <t>TIPOPRODUCTO_canasta (PK)</t>
+  </si>
+  <si>
+    <t>DESCRIPCION_canasta</t>
+  </si>
+  <si>
+    <t>IMAGEN_canasta</t>
+  </si>
+  <si>
+    <t>PRECIO_canasta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -190,24 +189,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,6 +330,286 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>83343</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>250031</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>226219</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51C2C3E3-7E2F-A2AD-03B2-A152686799D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4691062" y="1178719"/>
+          <a:ext cx="166688" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>511968</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726281</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>130969</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CuadroTexto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC4E5623-B89A-948C-FFE3-90FB083F565E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5119687" y="1774031"/>
+          <a:ext cx="214313" cy="261938"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>69056</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>354806</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>283369</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>45244</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CuadroTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFFF5C96-22D3-4501-82A7-2AF90DB61572}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7129462" y="1497806"/>
+          <a:ext cx="214313" cy="261938"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>661987</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>328613</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CuadroTexto 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0D8BA64-AEC0-4364-A601-6AF0DABB7483}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7722393" y="1209675"/>
+          <a:ext cx="214313" cy="261938"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>N</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -633,105 +911,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87261C84-CCC9-4D37-9AB7-6E67D0C83461}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E6" s="5" t="s">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E7" s="2" t="s">
+    <row r="7" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="8" t="s">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="2" t="s">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="3" t="s">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>13</v>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="4" t="s">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>